<commit_message>
source files for notes on reading and writing corrected
</commit_message>
<xml_diff>
--- a/content/manipulation_donnees/files/data_ex.xlsx
+++ b/content/manipulation_donnees/files/data_ex.xlsx
@@ -1,57 +1,359 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18915" windowHeight="11820"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="dataEx" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
-    <t xml:space="preserve">de1</t>
+    <t>de1</t>
   </si>
   <si>
-    <t xml:space="preserve">de2</t>
+    <t>de2</t>
   </si>
   <si>
-    <t xml:space="preserve">lanceur</t>
+    <t>lanceur</t>
   </si>
   <si>
-    <t xml:space="preserve">Luc</t>
+    <t>Luc</t>
   </si>
   <si>
-    <t xml:space="preserve">Kim</t>
+    <t>Kim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+  <fonts count="18" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -59,22 +361,217 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -119,6 +616,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -150,6 +651,10 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -351,14 +856,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -369,106 +874,104 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8"/>
       <c r="C8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
@@ -477,6 +980,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>